<commit_message>
SM and Cement notebooks
</commit_message>
<xml_diff>
--- a/Python2/Cheat_Sheet2.xlsx
+++ b/Python2/Cheat_Sheet2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/GSB/Documents/2024/CUNY/Python2/Python2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97AD3CB1-0F9B-FF44-B2CB-301F31CC7848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A374978E-2808-034E-AA24-0FEA992F1485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="1340" windowWidth="24180" windowHeight="17080" firstSheet="7" activeTab="12" xr2:uid="{78D90E6A-84B8-CE45-89A0-B6509A31357A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" firstSheet="7" activeTab="12" xr2:uid="{78D90E6A-84B8-CE45-89A0-B6509A31357A}"/>
   </bookViews>
   <sheets>
     <sheet name="Week1A" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4997" uniqueCount="2388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4999" uniqueCount="2390">
   <si>
     <t>Python Review</t>
   </si>
@@ -10050,12 +10050,78 @@
   <si>
     <t>df = pd.DataFrame(soup)</t>
   </si>
+  <si>
+    <t>df[…]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>df[...]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> syntax in pandas is commonly used to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>filter rows</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>select columns</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in a DataFrame.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="71">
+  <fonts count="73">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -10488,6 +10554,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -10712,7 +10792,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -10864,6 +10944,7 @@
     <xf numFmtId="0" fontId="70" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -25014,7 +25095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEBCF169-9633-E74D-B80D-F292D2186871}">
   <dimension ref="A1:F122"/>
   <sheetViews>
-    <sheetView topLeftCell="A118" workbookViewId="0">
+    <sheetView topLeftCell="A114" workbookViewId="0">
       <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
@@ -25709,15 +25790,16 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2756730-1ADB-AD4A-95D0-815E7B703BC7}">
-  <dimension ref="A1:A30"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:A30"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C30" sqref="C1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="24"/>
   <cols>
     <col min="1" max="1" width="81" style="113" customWidth="1"/>
+    <col min="2" max="2" width="108.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="27">
@@ -25816,6 +25898,14 @@
     <row r="30" spans="1:1">
       <c r="A30" s="113" t="s">
         <v>146</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="26">
+      <c r="A40" s="113" t="s">
+        <v>2388</v>
+      </c>
+      <c r="B40" s="121" t="s">
+        <v>2389</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SM pdf and Cheatsheet update
</commit_message>
<xml_diff>
--- a/Python2/Cheat_Sheet2.xlsx
+++ b/Python2/Cheat_Sheet2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/GSB/Documents/2024/CUNY/Python2/Python2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A374978E-2808-034E-AA24-0FEA992F1485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2011705-7D36-7649-8623-A9A3C4EF4E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" firstSheet="7" activeTab="12" xr2:uid="{78D90E6A-84B8-CE45-89A0-B6509A31357A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" firstSheet="7" activeTab="13" xr2:uid="{78D90E6A-84B8-CE45-89A0-B6509A31357A}"/>
   </bookViews>
   <sheets>
     <sheet name="Week1A" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4999" uniqueCount="2390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5002" uniqueCount="2393">
   <si>
     <t>Python Review</t>
   </si>
@@ -10116,12 +10116,118 @@
       <t xml:space="preserve"> in a DataFrame.</t>
     </r>
   </si>
+  <si>
+    <t>Formatting Numbers to Thousands</t>
+  </si>
+  <si>
+    <t>## format all tables</t>
+  </si>
+  <si>
+    <r>
+      <t>pd</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF212121"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF212121"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>options</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF212121"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF212121"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>display</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF212121"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF212121"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">float_format </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF212121"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF212121"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> '{:,.2f}'</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <color rgb="FF212121"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF212121"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>format</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="73">
+  <fonts count="76">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -10568,6 +10674,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF212121"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="13"/>
+      <color rgb="FF212121"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF212121"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -10792,7 +10918,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -10945,6 +11071,8 @@
     <xf numFmtId="0" fontId="70" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -25095,7 +25223,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEBCF169-9633-E74D-B80D-F292D2186871}">
   <dimension ref="A1:F122"/>
   <sheetViews>
-    <sheetView topLeftCell="A114" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
@@ -25792,7 +25920,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2756730-1ADB-AD4A-95D0-815E7B703BC7}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="C30" sqref="C1:F1048576"/>
     </sheetView>
   </sheetViews>
@@ -25916,12 +26044,32 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83940D90-E002-5E41-AD1D-635AD7E33F55}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="20">
+      <c r="A1" t="s">
+        <v>2390</v>
+      </c>
+      <c r="B1" s="122" t="s">
+        <v>2391</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="20">
+      <c r="B2" s="123" t="s">
+        <v>2392</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>